<commit_message>
Fixing a wrong row deletion
</commit_message>
<xml_diff>
--- a/collection.xlsx
+++ b/collection.xlsx
@@ -14016,11 +14016,11 @@
   <dimension ref="A1:V945"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4915" ySplit="555" topLeftCell="I34" activePane="bottomRight" state="split"/>
+      <pane xSplit="4915" ySplit="555" topLeftCell="I35" activePane="bottomRight" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
-      <selection pane="bottomRight" activeCell="I51" activeCellId="0" sqref="I51"/>
+      <selection pane="bottomLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
+      <selection pane="bottomRight" activeCell="P67" activeCellId="0" sqref="P67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -38505,11 +38505,11 @@
   <dimension ref="A1:L899"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D70" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D26" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A70" activeCellId="0" sqref="A70"/>
-      <selection pane="bottomRight" activeCell="H91" activeCellId="0" sqref="H91"/>
+      <selection pane="bottomLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+      <selection pane="bottomRight" activeCell="J47" activeCellId="0" sqref="J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -39991,7 +39991,7 @@
     </row>
     <row r="44" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="19" t="s">
-        <v>525</v>
+        <v>501</v>
       </c>
       <c r="B44" s="19"/>
       <c r="C44" s="32" t="s">
@@ -40009,7 +40009,6 @@
       <c r="G44" s="11" t="s">
         <v>507</v>
       </c>
-      <c r="H44" s="11"/>
       <c r="I44" s="41" t="n">
         <v>14</v>
       </c>

</xml_diff>